<commit_message>
Finished test cases v3
</commit_message>
<xml_diff>
--- a/Version3/test_cases_v3.xlsx
+++ b/Version3/test_cases_v3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0019c4aa09bcd7bb/Desktop/CPR Final/Version ^N3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0019c4aa09bcd7bb/Desktop/cprfinal - works/Version3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="695" documentId="8_{570DC9ED-5914-41BE-BB04-3B44D1E189F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D04F121-9F9D-40AE-B961-2BBBB95A517D}"/>
+  <xr:revisionPtr revIDLastSave="923" documentId="8_{570DC9ED-5914-41BE-BB04-3B44D1E189F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0407A6FC-BB14-4E68-B8F0-C431D8BC3405}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E9CD0BFC-551D-4216-AB69-D06DEB238C7B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="152">
   <si>
     <t>Cases Description</t>
   </si>
@@ -170,19 +170,346 @@
     <t>Block Name</t>
   </si>
   <si>
-    <t>Measuring</t>
-  </si>
-  <si>
     <t>Manipulating</t>
   </si>
   <si>
-    <t>Comparison</t>
-  </si>
-  <si>
-    <t>Converting to double</t>
-  </si>
-  <si>
-    <t>Tokenizing Phrases</t>
+    <t>Copying</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Use 'q' to quit</t>
+  </si>
+  <si>
+    <t>Should quit the current copying module</t>
+  </si>
+  <si>
+    <t>Quits the copying module</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Should not quit the current copying module</t>
+  </si>
+  <si>
+    <t>Does not quit the copying module</t>
+  </si>
+  <si>
+    <t>Give input wth leading white space</t>
+  </si>
+  <si>
+    <t>"    Hello"</t>
+  </si>
+  <si>
+    <t>Should ignore the leading white space</t>
+  </si>
+  <si>
+    <t>Does not ignore leading white space</t>
+  </si>
+  <si>
+    <t>gave no input</t>
+  </si>
+  <si>
+    <t>&lt;Enter&gt;</t>
+  </si>
+  <si>
+    <t>Should prompt user again for input</t>
+  </si>
+  <si>
+    <t>Accepts no input as input</t>
+  </si>
+  <si>
+    <t>Gave input with trailing white space</t>
+  </si>
+  <si>
+    <t>"Hello     "</t>
+  </si>
+  <si>
+    <t>Should ignore trailing white space</t>
+  </si>
+  <si>
+    <t>Does not ingore trailing whitespace</t>
+  </si>
+  <si>
+    <t>Gave a long string as 2nd input</t>
+  </si>
+  <si>
+    <t>bob, robert</t>
+  </si>
+  <si>
+    <t>robert</t>
+  </si>
+  <si>
+    <t>Gave a shorter string as 2nd input</t>
+  </si>
+  <si>
+    <t>robert, bob</t>
+  </si>
+  <si>
+    <t>bob</t>
+  </si>
+  <si>
+    <t>Gave integers as inputs</t>
+  </si>
+  <si>
+    <t>12345, 54321</t>
+  </si>
+  <si>
+    <t>Gave input starting with 'q'</t>
+  </si>
+  <si>
+    <t>quick</t>
+  </si>
+  <si>
+    <t>Should accpet and not quit module</t>
+  </si>
+  <si>
+    <t>does not quit module</t>
+  </si>
+  <si>
+    <t>Gave same string as input</t>
+  </si>
+  <si>
+    <t>bob, bob</t>
+  </si>
+  <si>
+    <t>"Please use a different string"</t>
+  </si>
+  <si>
+    <t>Searching</t>
+  </si>
+  <si>
+    <t>Should quit the current searching module</t>
+  </si>
+  <si>
+    <t>Should not quit the current searching module</t>
+  </si>
+  <si>
+    <t>Quits the searching module</t>
+  </si>
+  <si>
+    <t>Does not quit the searching module</t>
+  </si>
+  <si>
+    <t>"are" found at 6 position</t>
+  </si>
+  <si>
+    <t>"are" found at 10 position</t>
+  </si>
+  <si>
+    <t>"    Frogs are great",  "are"</t>
+  </si>
+  <si>
+    <t>"are" found at 5 position</t>
+  </si>
+  <si>
+    <t>"Cats are cool", "are   "</t>
+  </si>
+  <si>
+    <t>are not found</t>
+  </si>
+  <si>
+    <t>Gave input with a capital letter</t>
+  </si>
+  <si>
+    <t>"big goats", "goAts"</t>
+  </si>
+  <si>
+    <t>"goats" found at 5 position</t>
+  </si>
+  <si>
+    <t>goAts not found</t>
+  </si>
+  <si>
+    <t>Gave input with numbers</t>
+  </si>
+  <si>
+    <t>"123", "2"</t>
+  </si>
+  <si>
+    <t>2 found at 1 position</t>
+  </si>
+  <si>
+    <t>Gave input with no errors</t>
+  </si>
+  <si>
+    <t>"Hello world", "world"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"world" found at 6 position </t>
+  </si>
+  <si>
+    <t>gave input with symbols</t>
+  </si>
+  <si>
+    <t>"$%^&amp;", "&amp;"</t>
+  </si>
+  <si>
+    <t>&amp; found at 3 position</t>
+  </si>
+  <si>
+    <t>gave q as second input</t>
+  </si>
+  <si>
+    <t>"quiet", "q"</t>
+  </si>
+  <si>
+    <t>q found at 0 position</t>
+  </si>
+  <si>
+    <t>Converting to long</t>
+  </si>
+  <si>
+    <t>Gave letters as input</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>converted number is 0</t>
+  </si>
+  <si>
+    <t>Converted number is 25.000000</t>
+  </si>
+  <si>
+    <t>Gave number as input</t>
+  </si>
+  <si>
+    <t>Gave numbers with decimals as input</t>
+  </si>
+  <si>
+    <t>Gave symbols as input</t>
+  </si>
+  <si>
+    <t>#%$</t>
+  </si>
+  <si>
+    <t>Gave mixed numbers and letter input</t>
+  </si>
+  <si>
+    <t>1w2e</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Format specifier
+ is wrong in code.
+ %ld should be %lf</t>
+  </si>
+  <si>
+    <t>Gave negative numbers</t>
+  </si>
+  <si>
+    <t>Gave number between 1 and 0</t>
+  </si>
+  <si>
+    <t>".06"</t>
+  </si>
+  <si>
+    <t>Converted number Is 0.000000</t>
+  </si>
+  <si>
+    <t>Tokenizing Sentences</t>
+  </si>
+  <si>
+    <t>Should quit the Tokenizing Sentences module</t>
+  </si>
+  <si>
+    <t>Should not quit the Tokenizing Sentences module</t>
+  </si>
+  <si>
+    <t>Quits the Tokenizing Sentences module</t>
+  </si>
+  <si>
+    <t>Does not quit the Tokenizing Sentences module</t>
+  </si>
+  <si>
+    <t>Prompts user for input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gave 3 sentences seperated by a . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gave input with white spcae after the . </t>
+  </si>
+  <si>
+    <t>purple people. george bush. eggs eggs</t>
+  </si>
+  <si>
+    <t>purple people.george bush.eggs eggs</t>
+  </si>
+  <si>
+    <t>Sentence #1 is 'purple people'
+Sentence #2 is 'george bush'
+Sentence #3 is 'eggs eggs'</t>
+  </si>
+  <si>
+    <t>Sentence #1 is 'purple people'
+Sentence #2 is '  george bush'
+Sentence #3 is '  eggs eggs'</t>
+  </si>
+  <si>
+    <t>sent1.sent2</t>
+  </si>
+  <si>
+    <t>Sentence #1 is 'sent1'
+Sentence #2 is 'sent2'</t>
+  </si>
+  <si>
+    <t>Gave input with sybols</t>
+  </si>
+  <si>
+    <t>sent!.sent?</t>
+  </si>
+  <si>
+    <t>Sentence #1 is 'sent!'
+Sentence #2 is 'sent?'</t>
+  </si>
+  <si>
+    <t>Gave input with … as part of sentence</t>
+  </si>
+  <si>
+    <t>he…left.dog nose</t>
+  </si>
+  <si>
+    <t>Sentence #1 is 'he…left'
+Sentence #2 is 'dog nose'</t>
+  </si>
+  <si>
+    <t>Sentence #1 is 'he'
+Sentence #2 is 'left'
+Sentence #3 is 'dog nose'</t>
+  </si>
+  <si>
+    <t>Gave input starting with .</t>
+  </si>
+  <si>
+    <t>.hello.world</t>
+  </si>
+  <si>
+    <t>Sentence #1 is 'hello'
+Sentence #2 is 'world'</t>
+  </si>
+  <si>
+    <t>Gave input with spaces between .</t>
+  </si>
+  <si>
+    <t>he is. .the greatest. .turkey ever</t>
+  </si>
+  <si>
+    <t>Sentence #1 is 'he is'
+Sentence #2 is 'the greatest'
+Sentence #3 is 'turkey ever'</t>
+  </si>
+  <si>
+    <t>Sentence #1 is 'he is'
+Sentence #2 is ' '
+Sentence #3 is 'the greatest'
+Sentence #4 is ' '
+Sentence #5 is "turkey ever'</t>
   </si>
 </sst>
 </file>
@@ -226,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -240,6 +567,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,19 +907,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21C63BD-9345-471B-8702-388F8F46EC2A}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G51" sqref="C12:G51"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="56.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
     <col min="6" max="6" width="56.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -614,7 +945,9 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3"/>
+      <c r="H1" s="3" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -821,512 +1154,950 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="2">
+        <v>54321</v>
+      </c>
+      <c r="F19" s="2">
+        <v>54321</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>45</v>
-      </c>
       <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>16</v>
       </c>
       <c r="B32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
       <c r="B33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="2">
+        <v>25</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="2">
+        <v>25.99</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" s="2">
+        <v>-21</v>
+      </c>
+      <c r="E40" s="2">
+        <v>-21</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="2"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="2"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+        <v>124</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C52" s="2"/>

</xml_diff>